<commit_message>
updated scripts and record after the meeting
</commit_message>
<xml_diff>
--- a/record/Time and Payment.xlsx
+++ b/record/Time and Payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TOSHIBA3T/2022-09-07/Fortune500_SDG_Analysis/record/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D3FD14-C560-1C43-9761-F04C7CC347D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEBB5D9-2BF6-2646-A882-0FB1B5607381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="37700" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,10 +326,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -533,6 +533,21 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" s="2">
+        <v>44857</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.78333333333333333</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15-B15</f>
+        <v>7.4999999999999956E-2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
annual report and time and payment record update
</commit_message>
<xml_diff>
--- a/record/Time and Payment.xlsx
+++ b/record/Time and Payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Fortune500_SDG_Analysis\record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6408EBC0-D3A8-400A-BE6C-DE67F6223C41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166483D4-F702-4AE0-866A-983CF28ECF9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32380" yWindow="-1120" windowWidth="28220" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,8 +344,8 @@
   </sheetPr>
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
01_1keyword works! but improve
need to discuss 48~57是不是比較好
need to 看137以後用SDSN Keyword improve
整份code works
</commit_message>
<xml_diff>
--- a/record/Time and Payment.xlsx
+++ b/record/Time and Payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Fortune500_SDG_Analysis\record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04225997-953C-4352-8F3F-4D6DA9F8618C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0003F6F0-03A2-4443-9484-2264C19F5AE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32380" yWindow="-1120" windowWidth="28220" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -342,10 +342,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -789,7 +789,7 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" ref="D32:D38" si="2">C32-B32</f>
+        <f t="shared" ref="D32:D49" si="2">C32-B32</f>
         <v>6.944444444444442E-2</v>
       </c>
     </row>
@@ -897,6 +897,64 @@
       </c>
       <c r="C40" s="3">
         <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="2"/>
+        <v>3.9583333333333325E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D41" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D42" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D43" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D44" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D45" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D46" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D47" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D48" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" ht="15.75" customHeight="1">
+      <c r="D49" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
record add one hour
</commit_message>
<xml_diff>
--- a/record/Time and Payment.xlsx
+++ b/record/Time and Payment.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Fortune500_SDG_Analysis\record\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Fortune500_SDG_Analysis/record/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05462225-BCC7-4D81-A80A-19B0FF936F0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E960EDBB-6C2A-464C-AAE8-48913C02541B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32380" yWindow="-1120" windowWidth="28220" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -117,19 +129,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -345,15 +358,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -367,7 +380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>44811</v>
       </c>
@@ -382,7 +395,7 @@
         <v>9.7222222222222099E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -397,7 +410,7 @@
         <v>3.472222222222221E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>44815</v>
       </c>
@@ -412,7 +425,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>44821</v>
       </c>
@@ -427,7 +440,7 @@
         <v>6.6666666666666763E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>44824</v>
       </c>
@@ -442,7 +455,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>44828</v>
       </c>
@@ -457,7 +470,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>44829</v>
       </c>
@@ -472,12 +485,12 @@
         <v>9.7916666666666652E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>44836</v>
       </c>
@@ -492,7 +505,7 @@
         <v>0.15416666666666662</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>44836</v>
       </c>
@@ -507,7 +520,7 @@
         <v>6.944444444444442E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>44842</v>
       </c>
@@ -522,7 +535,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>44843</v>
       </c>
@@ -537,7 +550,7 @@
         <v>6.5972222222222099E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>44856</v>
       </c>
@@ -552,7 +565,7 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>44857</v>
       </c>
@@ -567,7 +580,7 @@
         <v>7.4999999999999956E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>44863</v>
       </c>
@@ -582,7 +595,7 @@
         <v>4.3750000000000011E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>44863</v>
       </c>
@@ -597,7 +610,7 @@
         <v>5.1388888888888817E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>44863</v>
       </c>
@@ -612,12 +625,12 @@
         <v>8.1249999999999933E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>44868</v>
       </c>
@@ -632,7 +645,7 @@
         <v>4.7222222222222165E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>44869</v>
       </c>
@@ -647,7 +660,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>44870</v>
       </c>
@@ -662,7 +675,7 @@
         <v>8.6111111111111138E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>44871</v>
       </c>
@@ -677,7 +690,7 @@
         <v>8.8888888888888906E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>44977</v>
       </c>
@@ -692,12 +705,12 @@
         <v>7.0833333333333304E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>44991</v>
       </c>
@@ -712,7 +725,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>44994</v>
       </c>
@@ -727,7 +740,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>45004</v>
       </c>
@@ -742,7 +755,7 @@
         <v>9.3055555555555558E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>45011</v>
       </c>
@@ -757,7 +770,7 @@
         <v>9.1666666666666563E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>45018</v>
       </c>
@@ -772,7 +785,7 @@
         <v>9.5138888888888884E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D31" s="3">
         <f>SUM(D26:D30)</f>
         <v>0.46736111111111101</v>
@@ -781,7 +794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>45032</v>
       </c>
@@ -792,11 +805,11 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" ref="D32:D51" si="2">C32-B32</f>
+        <f t="shared" ref="D32:D52" si="2">C32-B32</f>
         <v>6.944444444444442E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>45039</v>
       </c>
@@ -811,7 +824,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>45046</v>
       </c>
@@ -826,7 +839,7 @@
         <v>9.9999999999999978E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>45060</v>
       </c>
@@ -841,7 +854,7 @@
         <v>0.10277777777777763</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>45067</v>
       </c>
@@ -856,7 +869,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>45084</v>
       </c>
@@ -871,7 +884,7 @@
         <v>5.555555555555558E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8">
         <v>45096</v>
       </c>
@@ -886,12 +899,12 @@
         <v>7.0833333333333304E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>45100</v>
       </c>
@@ -906,7 +919,7 @@
         <v>3.9583333333333325E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>45108</v>
       </c>
@@ -921,7 +934,7 @@
         <v>0.13194444444444442</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>45116</v>
       </c>
@@ -936,7 +949,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>45138</v>
       </c>
@@ -951,7 +964,7 @@
         <v>0.10069444444444453</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>45158</v>
       </c>
@@ -966,7 +979,7 @@
         <v>7.638888888888884E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>45165</v>
       </c>
@@ -981,7 +994,7 @@
         <v>6.5972222222222099E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D46" s="3">
         <f>SUM(D40:D45)</f>
         <v>0.49791666666666656</v>
@@ -990,7 +1003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>45179</v>
       </c>
@@ -1005,7 +1018,7 @@
         <v>7.2916666666666741E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>45186</v>
       </c>
@@ -1020,7 +1033,7 @@
         <v>9.027777777777779E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>45193</v>
       </c>
@@ -1035,7 +1048,7 @@
         <v>9.2361111111111116E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>45200</v>
       </c>
@@ -1050,7 +1063,7 @@
         <v>9.027777777777779E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>45222</v>
       </c>
@@ -1063,6 +1076,21 @@
       <c r="D51" s="3">
         <f t="shared" si="2"/>
         <v>0.10347222222222219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="9">
+        <v>45224</v>
+      </c>
+      <c r="B52" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="2"/>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
time payment 22305元 update
</commit_message>
<xml_diff>
--- a/record/Time and Payment.xlsx
+++ b/record/Time and Payment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TOSHIBA EXT/4_teaching/repo/Fortune500_SDG_Analysis/record/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Fortune500_SDG_Analysis/record/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175381B-F740-514E-A162-D08117E1DE93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2C02A6-1762-5940-861F-6CC22851688B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36300" yWindow="-1160" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29100" yWindow="3580" windowWidth="38900" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -63,13 +67,21 @@
   </si>
   <si>
     <t>18000元 (paid)</t>
+  </si>
+  <si>
+    <t>14.87 hour</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>22305元</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -354,15 +366,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -376,7 +388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>44811</v>
       </c>
@@ -391,7 +403,7 @@
         <v>9.7222222222222099E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -406,7 +418,7 @@
         <v>3.472222222222221E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>44815</v>
       </c>
@@ -421,7 +433,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>44821</v>
       </c>
@@ -436,7 +448,7 @@
         <v>6.6666666666666763E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>44824</v>
       </c>
@@ -451,7 +463,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>44828</v>
       </c>
@@ -466,7 +478,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>44829</v>
       </c>
@@ -481,12 +493,12 @@
         <v>9.7916666666666652E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>44836</v>
       </c>
@@ -501,7 +513,7 @@
         <v>0.15416666666666662</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>44836</v>
       </c>
@@ -516,7 +528,7 @@
         <v>6.944444444444442E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>44842</v>
       </c>
@@ -531,7 +543,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>44843</v>
       </c>
@@ -546,7 +558,7 @@
         <v>6.5972222222222099E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>44856</v>
       </c>
@@ -561,7 +573,7 @@
         <v>3.8194444444444531E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>44857</v>
       </c>
@@ -576,7 +588,7 @@
         <v>7.4999999999999956E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>44863</v>
       </c>
@@ -591,7 +603,7 @@
         <v>4.3750000000000011E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>44863</v>
       </c>
@@ -606,7 +618,7 @@
         <v>5.1388888888888817E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>44863</v>
       </c>
@@ -621,12 +633,12 @@
         <v>8.1249999999999933E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>44868</v>
       </c>
@@ -641,7 +653,7 @@
         <v>4.7222222222222165E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>44869</v>
       </c>
@@ -656,7 +668,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>44870</v>
       </c>
@@ -671,7 +683,7 @@
         <v>8.6111111111111138E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>44871</v>
       </c>
@@ -686,7 +698,7 @@
         <v>8.8888888888888906E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>44977</v>
       </c>
@@ -701,12 +713,12 @@
         <v>7.0833333333333304E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>44991</v>
       </c>
@@ -721,7 +733,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>44994</v>
       </c>
@@ -736,7 +748,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>45004</v>
       </c>
@@ -751,7 +763,7 @@
         <v>9.3055555555555558E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>45011</v>
       </c>
@@ -766,7 +778,7 @@
         <v>9.1666666666666563E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>45018</v>
       </c>
@@ -781,7 +793,7 @@
         <v>9.5138888888888884E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D31" s="3">
         <f>SUM(D26:D30)</f>
         <v>0.46736111111111101</v>
@@ -790,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>45032</v>
       </c>
@@ -805,7 +817,7 @@
         <v>6.944444444444442E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>45039</v>
       </c>
@@ -820,7 +832,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>45046</v>
       </c>
@@ -835,7 +847,7 @@
         <v>9.9999999999999978E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>45060</v>
       </c>
@@ -850,7 +862,7 @@
         <v>0.10277777777777763</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>45067</v>
       </c>
@@ -865,7 +877,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>45084</v>
       </c>
@@ -880,7 +892,7 @@
         <v>5.555555555555558E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8">
         <v>45096</v>
       </c>
@@ -895,12 +907,12 @@
         <v>7.0833333333333304E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>45100</v>
       </c>
@@ -915,7 +927,7 @@
         <v>3.9583333333333325E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>45108</v>
       </c>
@@ -930,7 +942,7 @@
         <v>0.13194444444444442</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>45116</v>
       </c>
@@ -945,7 +957,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>45138</v>
       </c>
@@ -960,7 +972,7 @@
         <v>0.10069444444444453</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>45158</v>
       </c>
@@ -975,7 +987,7 @@
         <v>7.638888888888884E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>45165</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>6.5972222222222099E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D46" s="3">
         <f>SUM(D40:D45)</f>
         <v>0.49791666666666656</v>
@@ -999,7 +1011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>45179</v>
       </c>
@@ -1014,7 +1026,7 @@
         <v>7.2916666666666741E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>45186</v>
       </c>
@@ -1029,7 +1041,7 @@
         <v>9.027777777777779E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>45193</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>9.2361111111111116E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>45200</v>
       </c>
@@ -1059,7 +1071,7 @@
         <v>9.027777777777779E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>45222</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>0.10347222222222219</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="9">
         <v>45224</v>
       </c>
@@ -1089,7 +1101,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
         <v>45241</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>4.513888888888884E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
         <v>45242</v>
       </c>
@@ -1117,6 +1129,14 @@
       <c r="D54" s="3">
         <f t="shared" si="2"/>
         <v>8.3333333333333259E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heatmap adjustment, tutor time
</commit_message>
<xml_diff>
--- a/record/Time and Payment.xlsx
+++ b/record/Time and Payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Fortune500_SDG_Analysis/record/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6DB233-9D50-7F48-B167-45F7A273CB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7847BB-9608-C948-AE33-6367E8077202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31800" yWindow="1900" windowWidth="29440" windowHeight="19100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2445,9 +2445,15 @@
       <c r="E69" s="17"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
+      <c r="A70" s="19">
+        <v>45468</v>
+      </c>
+      <c r="B70" s="20">
+        <v>0.875</v>
+      </c>
+      <c r="C70" s="20">
+        <v>0.92222222222222217</v>
+      </c>
       <c r="D70" s="17"/>
       <c r="E70" s="17"/>
     </row>

</xml_diff>

<commit_message>
rerun change company and industry, and rerun result
</commit_message>
<xml_diff>
--- a/record/Time and Payment.xlsx
+++ b/record/Time and Payment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/Fortune500_SDG_Analysis/record/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B6D9F1-B230-7D42-91C8-5FE9C7352D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32AA583-A55B-3546-9A83-5834F566C171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="700" windowWidth="26040" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2471,9 +2471,15 @@
       <c r="E71" s="17"/>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
+      <c r="A72" s="19">
+        <v>45498</v>
+      </c>
+      <c r="B72" s="20">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C72" s="20">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="D72" s="17"/>
       <c r="E72" s="17"/>
     </row>

</xml_diff>